<commit_message>
Modificaciones de setters and getters
</commit_message>
<xml_diff>
--- a/src/test/resources/Datadriven/datosderegistro.xlsx
+++ b/src/test/resources/Datadriven/datosderegistro.xlsx
@@ -18,15 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
-    <t>Correo electronico</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Contrasena</t>
-  </si>
-  <si>
     <t>Alejandra</t>
   </si>
   <si>
@@ -39,13 +30,22 @@
     <t>Lolo*1994+</t>
   </si>
   <si>
-    <t>Nombre_tablero</t>
-  </si>
-  <si>
     <t>Prueba2</t>
   </si>
   <si>
     <t>Prueba3</t>
+  </si>
+  <si>
+    <t>correo electronico</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>contrasena</t>
+  </si>
+  <si>
+    <t>nombre_tablero</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -406,58 +406,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>